<commit_message>
Fix scripts 2, 3, 4 to use language config system
- Removed hardcoded Arabic paths and column names
- All 3 scripts now read language_config.txt dynamically
- Cleaned up 2_download_audio.py with improved error handling
- Deleted old Arabic Frequency Word List.xlsx
- Successfully downloaded 9/10 Malayalam audio files
</commit_message>
<xml_diff>
--- a/FluentForever_Malayalam_Perfect/working_data.xlsx
+++ b/FluentForever_Malayalam_Perfect/working_data.xlsx
@@ -540,7 +540,11 @@
           <t>He is with me.</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_02.mp3]</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -574,7 +578,11 @@
           <t>She danced along with the song.</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_03.mp3]</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -608,7 +616,11 @@
           <t>I need some money along with me.</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_04.mp3]</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -642,7 +654,11 @@
           <t>We played together.</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_05.mp3]</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -676,7 +692,11 @@
           <t>She walked with him.</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_06.mp3]</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -710,7 +730,11 @@
           <t>I took the pen along with the book.</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_07.mp3]</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -744,7 +768,11 @@
           <t>Will you come with me tomorrow?</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_08.mp3]</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -778,7 +806,11 @@
           <t>Father went to the shop with mother.</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_09.mp3]</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -812,7 +844,11 @@
           <t>She knew sadness along with happiness.</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_10.mp3]</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace Status with Sentences/Audio/Images count tracking
- Each word now tracked with counts (0-10) for each pipeline stage
- More robust error handling and partial completion tracking
- Scripts check counts instead of status strings
- Shows exact progress: Sentences=10/10 | Audio=5/10 | Images=10/10
- Batch processing respects BATCH_WORDS=5 default limit
</commit_message>
<xml_diff>
--- a/FluentForever_Malayalam_Perfect/working_data.xlsx
+++ b/FluentForever_Malayalam_Perfect/working_data.xlsx
@@ -506,8 +506,16 @@
           <t>I went with my mother.</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[sound:0003_ഒപ്പം_01.mp3]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_01.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -545,7 +553,11 @@
           <t>[sound:0003_ഒപ്പം_02.mp3]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_02.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -583,7 +595,11 @@
           <t>[sound:0003_ഒപ്പം_03.mp3]</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_03.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -621,7 +637,11 @@
           <t>[sound:0003_ഒപ്പം_04.mp3]</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_04.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -659,7 +679,11 @@
           <t>[sound:0003_ഒപ്പം_05.mp3]</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_05.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -697,7 +721,11 @@
           <t>[sound:0003_ഒപ്പം_06.mp3]</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_06.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -735,7 +763,11 @@
           <t>[sound:0003_ഒപ്പം_07.mp3]</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_07.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -773,7 +805,11 @@
           <t>[sound:0003_ഒപ്പം_08.mp3]</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_08.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -811,7 +847,11 @@
           <t>[sound:0003_ഒപ്പം_09.mp3]</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_09.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -849,7 +889,11 @@
           <t>[sound:0003_ഒപ്പം_10.mp3]</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>&lt;img src="0003_ഒപ്പം_10.jpg"&gt;</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor audio download to iterate through tracking file
- Changed from row-by-row iteration to tracking-file-based iteration
- Now correctly finds words needing audio based on Sentences/Audio counts
- Filters for rows with empty Sound column within each word
- Successfully tested: generated 10 sentences and downloaded 10 audio files for word 1
- Partial progress on word 2 (2/10) before network error
</commit_message>
<xml_diff>
--- a/FluentForever_Malayalam_Perfect/working_data.xlsx
+++ b/FluentForever_Malayalam_Perfect/working_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,422 +478,1062 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_01</t>
+          <t>0001_ദി_01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ഞാൻ അമ്മയുടെ ഒപ്പം പോയി.</t>
+          <t>ദി പുസ്തകം എവിടെ?</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>/ɲaːn̪ amːɐjuːʈe oːpːam poːji/</t>
+          <t>/di pustakam eviṭe?/</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>I went with my mother.</t>
+          <t>Where is the book?</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_01.mp3]</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_01.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_01.mp3]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_02</t>
+          <t>0001_ദി_02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>അവൻ എന്റെ ഒപ്പം ഉണ്ട്.</t>
+          <t>ദി ആൾ നല്ലവൻ ആണ്.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>/ɐʋɐn en̪d̪e oːpːam uɳʈɨ/</t>
+          <t>/di aaḷ nallavan aaṇ./</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>He is with me.</t>
+          <t>The man is good.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_02.mp3]</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_02.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_02.mp3]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_03</t>
+          <t>0001_ദി_03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>അവൾ പാട്ടിന്റെ ഒപ്പം നൃത്തം ചെയ്തു.</t>
+          <t>ഞാൻ ദി സിനിമ കണ്ടു.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>/ɐʋɐɭ paːʈːin̪t̪e oːpːam n̪r̥t̪ːam t͡ʃeɪ̯t̪u/</t>
+          <t>/ɲaan di sinima kaṇṭu./</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>She danced along with the song.</t>
+          <t>I saw the movie.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_03.mp3]</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_03.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_03.mp3]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_04</t>
+          <t>0001_ദി_04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>എനിക്ക് കുറച്ച് പണം ഒപ്പം വേണം.</t>
+          <t>അവൾ ദി പാട്ട് പാടി.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>/enɪkːɨ kʊrɐt͡ʃːɨ paɳɐm oːpːam ʋeːɳɐm/</t>
+          <t>/avaḷ di paatt paati./</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>I need some money along with me.</t>
+          <t>She sang the song.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_04.mp3]</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_04.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_04.mp3]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_05</t>
+          <t>0001_ദി_05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ഞങ്ങൾ ഒപ്പം കളിച്ചു.</t>
+          <t>ഇത് ദി വീട് ആണ്.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>/ɲɐŋŋɐɭ oːpːam kɐɭɪt͡ʃːu/</t>
+          <t>/ith di veet aahn./</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>We played together.</t>
+          <t>This is the house.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_05.mp3]</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_05.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_05.mp3]</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_06</t>
+          <t>0001_ദി_06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>അവൾ അവന്റെ ഒപ്പം നടന്നു.</t>
+          <t>ദി പരീക്ഷ അടുത്ത ആഴ്ച ആണ്.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>/ɐʋɐɭ ɐʋɐn̪d̪e oːpːam nɐɖɐn̪n̪u/</t>
+          <t>/di pareekṣa aṭutta aazhcha aaṇ./</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>She walked with him.</t>
+          <t>The exam is next week.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_06.mp3]</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_06.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_06.mp3]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_07</t>
+          <t>0001_ദി_07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>പുസ്തകത്തിന്റെ ഒപ്പം പേനയും എടുത്തു.</t>
+          <t>അവൻ ദി പണം കൊടുത്തു.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>/pust̪ɐkɐt̪ːin̪d̪e oːpːam peːn̪ɐjum ed̪ut̪t̪u/</t>
+          <t>/avan di paṇam koṭuttu./</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>I took the pen along with the book.</t>
+          <t>He gave the money.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_07.mp3]</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_07.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_07.mp3]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_08</t>
+          <t>0001_ദി_08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>നാളെ നീ എന്റെ ഒപ്പം വരുമോ?</t>
+          <t>അമ്മ ദി ഭക്ഷണം ഉണ്ടാക്കി.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>/n̪aːɭe n̪iː en̪d̪e oːpːam ʋɐɾumoː/</t>
+          <t>/amma di bhaക്ഷണം uṇṭaakki./</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Will you come with me tomorrow?</t>
+          <t>Mother made the food.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_08.mp3]</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_08.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_08.mp3]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0003_ഒപ്പം_09</t>
+          <t>0001_ദി_09</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ഒപ്പം</t>
+          <t>ദി</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>അച്ഛൻ അമ്മയുടെ ഒപ്പം കടയിൽ പോയി.</t>
+          <t>ഞങ്ങൾ ദി സ്ഥലം കണ്ടു.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>/ɐt͡ʃːʰɐn amːɐjuːʈe oːpːam kɐɖɐjil poːji/</t>
+          <t>/ɲaṅṅaḷ di sthalam kaṇṭu./</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Father went to the shop with mother.</t>
+          <t>We saw the place.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[sound:0003_ഒപ്പം_09.mp3]</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_09.jpg"&gt;</t>
-        </is>
-      </c>
+          <t>[sound:0001_ദി_09.mp3]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>0001_ദി_10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ദി</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The word 'ദി' (di) is a definite article in Malayalam, equivalent to 'the' in English. It specifies a particular noun.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ഇതാണ് ദി വഴി വീട്ടിലേക്ക്.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>/ithaahn di vazhi veettilekk./</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>This is the way home.</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[sound:0001_ദി_10.mp3]</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_01</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>അത് ശരിയായിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>/ɐt̪ɨ̆ ʃɐɾiyɐːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>That might be right.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_02</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>അവൻ നാളെ വരും, ആയിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>/ɐʋɐn̪ naːɭe ʋɐɾum, aːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>He will come tomorrow, maybe.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_03</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>അവൾക്ക് സന്തോഷം ആയിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>/ɐʋɐɭkːɨ̆ saⁿt̪oːʃɐm aːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>She will be happy.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>അത് എളുപ്പമായിരിക്കും എന്ന് തോന്നുന്നു.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>/ɐt̪ɨ̆ eɭuppɐmaːyirikkum ennɨ t̪oːnnunnu/</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>It seems like it might be easy.</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_05</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>നാളെ മഴ പെയ്യാൻ സാധ്യതയുണ്ട്, ആയിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>/naːɭe mɐɻɐ peyyɐːn̪ saːd̪͡ʱjɐt̪ɐjuɳɖɨ̆, aːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>There is a chance of rain tomorrow, maybe.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_06</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>അവർക്ക് അത് അറിയാമായിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>/ɐʋɐrkːɨ̆ ɐt̪ɨ̆ ɐɾiyaːmaːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>They probably know it.</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_07</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>അവൻ ഒരു ഡോക്ടർ ആയിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>/ɐʋɐn̪ oɾu ɖoːkːt̪ɐr aːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>He might be a doctor.</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_08</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>അവർ വൈകി വരും, ആയിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>/ɐʋɐr ʋɐiki ʋɐɾum, aːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>They might come late.</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_09</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ഈ സിനിമ നല്ലതായിരിക്കും എന്ന് കരുതുന്നു.</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>/iː sinimɐ nɐllɐt̪aːyirikkum ennɨ kɐɾut̪unnɨ/</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>I think this movie might be good.</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0002_ആയിരിക്കും_10</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ആയിരിക്കും</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>"ആയിരിക്കും" (aayirikkum) means "will be" or "might be" in English. It expresses possibility, likelihood, or future tense with a degree of uncertainty.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>അത് ഒരു നല്ല തീരുമാനം ആയിരിക്കും.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>/ɐt̪ɨ̆ oɾu nɐllɐ t̪iːɾumaːnɐm aːyirikkum/</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>That might be a good decision.</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ഞാൻ അമ്മയുടെ ഒപ്പം പോയി.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>/ɲaːn̪ ɐmːɐjuːɖeː oppɐm poːyiː/</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>I went with my mother.</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_02</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>അവൻ എന്റെ ഒപ്പം ഉണ്ട്.</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>/ɐʋɐn̪ endeː oppɐm uɳɖɨ̆/</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>He is with me.</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_03</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>അവൾ അവന്റെ ഒപ്പം കളിച്ചു.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>/ɐʋɐɭ ɐʋɐn̪deː oppɐm kɐɭit͡ʃːu/</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>She played with him.</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>അവർ ഒപ്പം നടന്നു.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>/ɐʋɐr oppɐm nɐɖɐn̪n̪u/</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>They walked together.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_05</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>എനിക്ക് ഒരു പേന ഒപ്പം ഒരു പുസ്തകവും വേണം.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>/enikːɨ̆ oru peːnɐ oppɐm oru pustɐkɐvum veːɳɐm/</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>I need a pen along with a book.</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_06</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>അച്ഛൻ എന്റെ ഒപ്പം വരും.</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>/ɐt͡ʃːʰɐn̪ endeː oppɐm vɐrum/</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Father will come with me.</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_07</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>അവൾ പാട്ടുപാടി, ഒപ്പം നൃത്തം ചെയ്തു.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>/ɐʋɐɭ paːt̪ːɨ̆ paːɖi oppɐm nrɨt̪ːɐm t͡ʃeːyt͡ʃu/</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>She sang and danced as well.</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_08</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>പരീക്ഷ ഒപ്പം പഠനം പ്രധാനമാണ്.</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>/pɐriːkʂɐ oppɐm pɐɖɐnɐm prɐd͡ʒʰaːnɐmaːɳɨ̆/</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Exams and studies are important.</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0003_ഒപ്പം_09</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ഒപ്പം</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>ഞങ്ങൾ ഒപ്പം സിനിമക്ക് പോയിരുന്നു.</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>/ɲɐŋŋɐɭ oppɐm sinimɐkːɨ̆ poːyirun̪n̪u/</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>We had gone to the cinema together.</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>0003_ഒപ്പം_10</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>ഒപ്പം</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>"ഒപ്പം" (Oppam) means "together with", "along with", or "besides" in English. It indicates accompaniment or being in association with something or someone.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>അവൾ സന്തോഷത്തിന്റെ ഒപ്പം വിഷമവും അറിഞ്ഞു.</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>/ɐʋɐɭ sɐn̪t̪oːʃɐt̪ːin̪d̪e oːpːam ʋɪʃɐmɐʋum ɐrɪɲ͡ɲu/</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>She knew sadness along with happiness.</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>[sound:0003_ഒപ്പം_10.mp3]</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>&lt;img src="0003_ഒപ്പം_10.jpg"&gt;</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>"ഒപ്പം" (Oppam) in Malayalam means "together with," "along with," or "besides."</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>അവൻ എന്നെ ഒപ്പം കൂട്ടാൻ പറഞ്ഞു.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>/ɐʋɐn̪ enneː oppɐm kuːt̪ːaːn̪ pɐrɐɲːu/</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>He asked me to join (him).</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>